<commit_message>
updated python scripts for collapsible and textblock detection
</commit_message>
<xml_diff>
--- a/GetTextBlockHtml/input.xlsx
+++ b/GetTextBlockHtml/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1220" yWindow="760" windowWidth="29020" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1420" yWindow="760" windowWidth="28820" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="1" state="visible" r:id="rId1"/>
@@ -460,8 +460,8 @@
   </sheetPr>
   <dimension ref="A1:B3023"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -483,151 +483,107 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>https://www.american.edu/about/strategic-plan/2019/index.cfm</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/index.cfm</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/accept-your-offer/index.cfm</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/admissions/rsvp/index.cfm</t>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/sustainability-competitions.cfm</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/adjudication.cfm</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/about/sustainability/sustainability-plan/sustainability-plan-administration.cfm</t>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/code.cfm</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/about/sustainability/sustainability-symposium.cfm</t>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/faculty.cfm</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/about/sustainability/sustainable-move-in.cfm</t>
-        </is>
-      </c>
+      <c r="B12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/about/sustainability/tracking-progress.cfm</t>
-        </is>
-      </c>
+      <c r="B13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/about/sustainability/tracking-progress/index.cfm</t>
-        </is>
-      </c>
+      <c r="B14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/about/visiting-campus.cfm</t>
-        </is>
-      </c>
+      <c r="B15" s="2" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/abroadatau/index.cfm</t>
-        </is>
-      </c>
+      <c r="B16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/complaint-process.cfm</t>
-        </is>
-      </c>
+      <c r="B17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/courses-registration.cfm</t>
-        </is>
-      </c>
+      <c r="B18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/integrity/adjudication.cfm</t>
-        </is>
-      </c>
+      <c r="B19" s="2" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/integrity/cheating.cfm</t>
-        </is>
-      </c>
+      <c r="B20" s="2" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/integrity/code.cfm</t>
-        </is>
-      </c>
+      <c r="B21" s="2" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>https://www.american.edu/academics/integrity/contacts.cfm</t>
-        </is>
-      </c>
+      <c r="B22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="B23" s="2" t="n"/>
@@ -9135,6 +9091,11 @@
     <row r="3024" ht="16" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:A3026"/>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B9" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B11" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader/>
@@ -9153,7 +9114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9351,12 +9312,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/index.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>txt-4676934</t>
+          <t>txt-5675573</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -9368,12 +9329,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/index.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>txt-4689167</t>
+          <t>txt-5674890</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -9385,97 +9346,97 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.american.edu/accept-your-offer/index.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>txt-6912491</t>
+          <t>cs_control_5674895-collapse</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.american.edu/accept-your-offer/index.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>txt-6914248</t>
+          <t>cs_control_5674921-collapse</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.american.edu/admissions/rsvp/index.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>congratulations-on-your-admission-to-american-university-</t>
+          <t>cs_control_5674922-collapse</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>txt-6946120</t>
+          <t>cs_control_5674924-collapse</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>arts-amp-sciences</t>
+          <t>cs_control_5674958-collapse</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/centers/antiracism/thinking-freedom-series.cfm</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>business-amp-economy</t>
+          <t>txt-5691872</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -9487,12 +9448,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>entertainment-amp-media</t>
+          <t>implementation-teams</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -9504,29 +9465,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>government-politics--amp-law</t>
+          <t>txt-5433017</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>nonprofits</t>
+          <t>txt-5433068</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -9538,46 +9499,46 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>sports</t>
+          <t>txt-5433019</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.american.edu/alumni/about/notable-alumni.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>txt-7023897</t>
+          <t>txt-5433021</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>au-arts</t>
+          <t>txt-5433055</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -9589,46 +9550,46 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>txt-7048737</t>
+          <t>txt-5429100</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/strategic-plan/2019/team.cfm</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>txt-7091559</t>
+          <t>txt-5429101</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>txt-7091565</t>
+          <t>we-39-re-on-our-way-to-zero-waste</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -9640,12 +9601,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>txt-7065144</t>
+          <t>txt-4635685</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -9657,29 +9618,29 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>txt-7065146</t>
+          <t>txt-4704895</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>txt-7065145</t>
+          <t>txt-4704907</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -9691,12 +9652,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>txt-7065149</t>
+          <t>txt-4781701</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -9708,12 +9669,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>txt-7065503</t>
+          <t>txt-4781709</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -9725,12 +9686,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>txt-7065508</t>
+          <t>txt-4781757</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -9742,12 +9703,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.american.edu/arts/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>txt-7065154</t>
+          <t>txt-4781805</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -9759,29 +9720,29 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>txt-6796300</t>
+          <t>txt-4704949</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>txt-6832485</t>
+          <t>cs_control_5524586-collapse</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -9793,12 +9754,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>txt-6796104</t>
+          <t>cs_control_5524587-collapse</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -9810,29 +9771,29 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>txt-6799430</t>
+          <t>cs_control_5524591-collapse</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/campus-greening/waste.cfm</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>txt-6832596</t>
+          <t>txt-6877899</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -9844,12 +9805,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/about/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>txt-6834665</t>
+          <t>txt-4613598</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -9861,12 +9822,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>txt-6899815</t>
+          <t>txt-6836132</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -9878,12 +9839,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>txt-6837609</t>
+          <t>txt-6836140</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -9895,12 +9856,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>txt-6899878</t>
+          <t>txt-6836112</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -9912,46 +9873,46 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>txt-6899876</t>
+          <t>txt-5734209</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>txt-6899431</t>
+          <t>txt-5507286</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>txt-6899799</t>
+          <t>txt-5507288</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -9963,12 +9924,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>txt-6899343</t>
+          <t>txt-5734729</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -9980,12 +9941,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>txt-6899855</t>
+          <t>txt-5507298</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -9997,46 +9958,46 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.american.edu/cas/anthropology/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>txt-6899848</t>
+          <t>txt-5507289</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/sustainability-plan/sustainability-plan-administration.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>administration</t>
+          <t>txt-5507290</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/sustainability-symposium.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>au-sustainability-symposium</t>
+          <t>txt-5507299</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -10048,12 +10009,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/sustainability-symposium.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>agenda</t>
+          <t>txt-5507300</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -10065,12 +10026,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/sustainable-move-in.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>txt-7031891</t>
+          <t>txt-5514819</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -10082,12 +10043,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/sustainable-move-in.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>sustainability-at-all-american-welcome</t>
+          <t>txt-5515495</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -10099,12 +10060,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/tracking-progress.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>tracking-progress</t>
+          <t>txt-5507320</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -10116,12 +10077,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/tracking-progress.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>greenhouse-gas-emissions</t>
+          <t>txt-5507301</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -10133,12 +10094,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/tracking-progress.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>txt-4986610</t>
+          <t>txt-5507422</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -10150,29 +10111,29 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/sustainability/tracking-progress/index.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>sustainability-dashboard</t>
+          <t>txt-5515486</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/visiting-campus.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>visit-au</t>
+          <t>txt-5515488</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -10184,12 +10145,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.american.edu/about/visiting-campus.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>txt-5176697</t>
+          <t>txt-5515519</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -10201,12 +10162,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/complaint-process.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>complaint-process-information</t>
+          <t>txt-5515510</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -10218,12 +10179,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/courses-registration.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>courses-and-registration</t>
+          <t>txt-5507331</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -10235,12 +10196,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/adjudication.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>adjudication-process</t>
+          <t>txt-5515472</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -10252,12 +10213,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/cheating.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>cheating</t>
+          <t>txt-5507347</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -10269,12 +10230,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>academic-integrity-code</t>
+          <t>txt-5515525</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -10286,12 +10247,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>watch-academic-integrity-videos</t>
+          <t>txt-5515513</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -10303,12 +10264,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>txt-5644841</t>
+          <t>txt-5515465</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -10320,34 +10281,493 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>txt-5644844</t>
+          <t>txt-5507353</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.american.edu/academics/integrity/contacts.cfm</t>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>contacts</t>
+          <t>txt-5507380</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/milestones.cfm</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>txt-5515532</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>benefits-of-reusable-water-bottles</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>dc-water</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>cs_control_6346253-collapse</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>cs_control_6361607-collapse</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>cs_control_6346259-collapse</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>cs_control_6346261-collapse</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>cs_control_6361592-collapse</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>cs_control_6346274-collapse</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>cs_control_6346263-collapse</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>cs_control_6361600-collapse</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>cs_control_6346271-collapse</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>cs_control_6346279-collapse</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>cs_control_6361613-collapse</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>cs_control_6346252-collapse</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>cs_control_6346257-collapse</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/plastic-reduction.cfm</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>cs_control_6346269-collapse</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/sustainability-competitions.cfm</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>campus-race-to-zero-waste</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/sustainability-competitions.cfm</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>cs_control_5896649-collapse</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/sustainability-competitions.cfm</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>cs_control_5896651-collapse</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/about/sustainability/sustainability-competitions.cfm</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>cs_control_5948475-collapse</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/adjudication.cfm</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>adjudication-process</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>academic-integrity-code</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>watch-academic-integrity-videos</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>txt-5644841</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/code.cfm</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>txt-5644844</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>https://www.american.edu/academics/integrity/faculty.cfm</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>faculty-resources</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>✅</t>
         </is>
       </c>
     </row>

</xml_diff>